<commit_message>
Revert "Accreditamento per A1#111#CGMX1-DFD-COMPUGROUP_MEDICAL_ITALIA_S.R.L-4.40"
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111#CGMX1/COMPUGROUP_MEDICAL_ITALIA_S.R.L/DFD/4.40/report-checklist.xlsx
+++ b/GATEWAY/A1#111#CGMX1/COMPUGROUP_MEDICAL_ITALIA_S.R.L/DFD/4.40/report-checklist.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29602"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cgm01-my.sharepoint.com/personal/giuseppe_carlino_cgm_com/Documents/FSE 2.0/Accreditamenti/DFD/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9D163366-D50A-4FFF-B573-C569523A22E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{32536F64-56C4-47E6-A8B3-83CE997AE18A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-12120" windowWidth="38640" windowHeight="21120" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1108" uniqueCount="469">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1107" uniqueCount="468">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -1670,16 +1670,13 @@
 </t>
   </si>
   <si>
-    <t>17/12/2025</t>
-  </si>
-  <si>
-    <t>2025-12-17T10:44:33Z</t>
-  </si>
-  <si>
-    <t>b8579c8591ee97fd238760f632f4adc5</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.190.4.4.31dbb846c23693b98c0e49ba7a3ac70e9c948fefac4ca292a09cf1286221383b.65007782fb^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2025-12-15T12:31:18Z</t>
+  </si>
+  <si>
+    <t>5b1a263b367d3be3d0297c12eacffd78</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190.4.4.ed2b07875251fa4f8740937f890453531ee2109e321fa1c45b01f9ba686eae8f.504872cb19^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_PSS_CT24</t>
@@ -2408,15 +2405,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="17" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2431,6 +2419,15 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="17" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -3896,8 +3893,8 @@
   <dimension ref="A1:W750"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="E191" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="G3" sqref="G3"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="G138" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="E193" sqref="E193"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
     </sheetView>
@@ -3941,11 +3938,11 @@
       <c r="W1" s="9"/>
     </row>
     <row r="2" spans="1:23" ht="14.25" customHeight="1">
-      <c r="A2" s="50" t="s">
+      <c r="A2" s="47" t="s">
         <v>18</v>
       </c>
       <c r="B2" s="54"/>
-      <c r="C2" s="51" t="s">
+      <c r="C2" s="48" t="s">
         <v>19</v>
       </c>
       <c r="D2" s="54"/>
@@ -3969,11 +3966,11 @@
       <c r="W2" s="9"/>
     </row>
     <row r="3" spans="1:23" ht="14.25" customHeight="1">
-      <c r="A3" s="52" t="s">
+      <c r="A3" s="49" t="s">
         <v>20</v>
       </c>
       <c r="B3" s="55"/>
-      <c r="C3" s="53" t="s">
+      <c r="C3" s="50" t="s">
         <v>21</v>
       </c>
       <c r="D3" s="54"/>
@@ -3999,7 +3996,7 @@
     <row r="4" spans="1:23" ht="14.25" customHeight="1">
       <c r="A4" s="56"/>
       <c r="B4" s="57"/>
-      <c r="C4" s="53" t="s">
+      <c r="C4" s="50" t="s">
         <v>22</v>
       </c>
       <c r="D4" s="54"/>
@@ -4026,7 +4023,7 @@
     <row r="5" spans="1:23" ht="14.25" customHeight="1">
       <c r="A5" s="58"/>
       <c r="B5" s="59"/>
-      <c r="C5" s="53" t="s">
+      <c r="C5" s="50" t="s">
         <v>23</v>
       </c>
       <c r="D5" s="54"/>
@@ -4050,7 +4047,7 @@
       <c r="W5" s="9"/>
     </row>
     <row r="6" spans="1:23" ht="14.25" customHeight="1">
-      <c r="A6" s="49"/>
+      <c r="A6" s="46"/>
       <c r="B6" s="60"/>
       <c r="C6" s="10"/>
       <c r="F6" s="6"/>
@@ -11039,19 +11036,19 @@
       <c r="E191" s="43" t="s">
         <v>422</v>
       </c>
-      <c r="F191" s="46" t="s">
+      <c r="F191" s="51">
+        <v>46006</v>
+      </c>
+      <c r="G191" s="52" t="s">
         <v>423</v>
       </c>
-      <c r="G191" s="47" t="s">
+      <c r="H191" s="52" t="s">
         <v>424</v>
       </c>
-      <c r="H191" s="47" t="s">
+      <c r="I191" s="52" t="s">
         <v>425</v>
       </c>
-      <c r="I191" s="47" t="s">
-        <v>426</v>
-      </c>
-      <c r="J191" s="48" t="s">
+      <c r="J191" s="53" t="s">
         <v>84</v>
       </c>
       <c r="K191" s="38"/>
@@ -11081,10 +11078,10 @@
         <v>57</v>
       </c>
       <c r="D192" s="35" t="s">
+        <v>426</v>
+      </c>
+      <c r="E192" s="43" t="s">
         <v>427</v>
-      </c>
-      <c r="E192" s="43" t="s">
-        <v>428</v>
       </c>
       <c r="F192" s="37"/>
       <c r="G192" s="37"/>
@@ -11097,7 +11094,7 @@
         <v>60</v>
       </c>
       <c r="L192" s="38" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="M192" s="38"/>
       <c r="N192" s="38"/>
@@ -11124,10 +11121,10 @@
         <v>57</v>
       </c>
       <c r="D193" s="35" t="s">
+        <v>429</v>
+      </c>
+      <c r="E193" s="44" t="s">
         <v>430</v>
-      </c>
-      <c r="E193" s="44" t="s">
-        <v>431</v>
       </c>
       <c r="F193" s="37"/>
       <c r="G193" s="37"/>
@@ -11140,7 +11137,7 @@
         <v>60</v>
       </c>
       <c r="L193" s="38" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="M193" s="38"/>
       <c r="N193" s="38"/>
@@ -15175,37 +15172,37 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="8" spans="1:1">
@@ -15243,22 +15240,22 @@
   <sheetData>
     <row r="1" spans="1:7" ht="14.25" customHeight="1" thickBot="1">
       <c r="A1" s="29" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>25</v>
       </c>
       <c r="C1" s="11" t="s">
+        <v>440</v>
+      </c>
+      <c r="D1" s="11" t="s">
         <v>441</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="F1" s="15" t="s">
         <v>442</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="G1" s="14" t="s">
         <v>443</v>
-      </c>
-      <c r="G1" s="14" t="s">
-        <v>444</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="14.25" customHeight="1">
@@ -15266,13 +15263,13 @@
         <v>48</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>444</v>
+      </c>
+      <c r="C2" s="12" t="s">
         <v>445</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="D2" s="30" t="s">
         <v>446</v>
-      </c>
-      <c r="D2" s="30" t="s">
-        <v>447</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="14.25" customHeight="1">
@@ -15280,13 +15277,13 @@
         <v>55</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="C3" s="12" t="s">
+        <v>447</v>
+      </c>
+      <c r="D3" s="30" t="s">
         <v>448</v>
-      </c>
-      <c r="D3" s="30" t="s">
-        <v>449</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="14.25" customHeight="1">
@@ -15294,13 +15291,13 @@
         <v>62</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="C4" s="12" t="s">
+        <v>449</v>
+      </c>
+      <c r="D4" s="31" t="s">
         <v>450</v>
-      </c>
-      <c r="D4" s="31" t="s">
-        <v>451</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="14.25" customHeight="1">
@@ -15308,13 +15305,13 @@
         <v>66</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="C5" s="12" t="s">
+        <v>451</v>
+      </c>
+      <c r="D5" s="30" t="s">
         <v>452</v>
-      </c>
-      <c r="D5" s="30" t="s">
-        <v>453</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="14.25" customHeight="1">
@@ -15322,13 +15319,13 @@
         <v>68</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="C6" s="12" t="s">
+        <v>453</v>
+      </c>
+      <c r="D6" s="31" t="s">
         <v>454</v>
-      </c>
-      <c r="D6" s="31" t="s">
-        <v>455</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="14.45">
@@ -15336,13 +15333,13 @@
         <v>70</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="C7" s="12" t="s">
+        <v>455</v>
+      </c>
+      <c r="D7" s="31" t="s">
         <v>456</v>
-      </c>
-      <c r="D7" s="31" t="s">
-        <v>457</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="14.45">
@@ -15350,13 +15347,13 @@
         <v>64</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="C8" s="12" t="s">
+        <v>457</v>
+      </c>
+      <c r="D8" s="31" t="s">
         <v>458</v>
-      </c>
-      <c r="D8" s="31" t="s">
-        <v>459</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="14.45">
@@ -15364,27 +15361,27 @@
         <v>57</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="C9" s="12" t="s">
+        <v>459</v>
+      </c>
+      <c r="D9" s="31" t="s">
         <v>460</v>
-      </c>
-      <c r="D9" s="31" t="s">
-        <v>461</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="43.15">
       <c r="A10" s="5" t="s">
+        <v>461</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>444</v>
+      </c>
+      <c r="C10" s="13" t="s">
         <v>462</v>
       </c>
-      <c r="B10" s="5" t="s">
-        <v>445</v>
-      </c>
-      <c r="C10" s="13" t="s">
+      <c r="D10" s="30" t="s">
         <v>463</v>
-      </c>
-      <c r="D10" s="30" t="s">
-        <v>464</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="14.25" customHeight="1">
@@ -15392,13 +15389,13 @@
         <v>335</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="C11" s="12" t="s">
+        <v>464</v>
+      </c>
+      <c r="D11" s="31" t="s">
         <v>465</v>
-      </c>
-      <c r="D11" s="31" t="s">
-        <v>466</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="14.25" customHeight="1">
@@ -16387,7 +16384,7 @@
     </row>
     <row r="2" spans="1:2" ht="14.25" customHeight="1">
       <c r="A2" s="4" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>84</v>
@@ -16395,7 +16392,7 @@
     </row>
     <row r="3" spans="1:2" ht="14.25" customHeight="1">
       <c r="A3" s="4" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>59</v>
@@ -17415,6 +17412,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -17423,7 +17426,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100BE9A258ADBC3EC4CBEB1E2AB9909207A" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0284f501378927579289f00316ec8a74">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="295b7897-c886-40bf-9750-5782b814c3e4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b47213d65be806e283915cff374a7eef" ns2:_="">
     <xsd:import namespace="295b7897-c886-40bf-9750-5782b814c3e4"/>
@@ -17567,22 +17570,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}"/>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}"/>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7568E770-0BC4-46AF-B6C6-958AE21C8F7F}"/>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}"/>
 </file>
 
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>